<commit_message>
CoSES: write variable prices as forecasts, read and write the files in cycles
</commit_message>
<xml_diff>
--- a/CoSES/data/Test1_Last_Preise.xlsx
+++ b/CoSES/data/Test1_Last_Preise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Arbeitsordner_MEMAP\02_Interface_OPCUA_Server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B75281-DFC7-45AA-838D-9C4CEDD6240E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DCDC94-E6D2-4FE5-9CBA-3B1C6EB01863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1650" yWindow="1695" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wärme" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Zeitschritt</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Periodendauer</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
@@ -118,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +138,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -201,7 +219,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Kosten!$C$3:$C$34</c:f>
+              <c:f>Kosten!$C$4:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="32"/>
@@ -306,7 +324,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Wärme!$F$3:$F$34</c:f>
+              <c:f>Wärme!$F$4:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -466,7 +484,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Kosten!$C$3:$C$34</c:f>
+              <c:f>Kosten!$C$4:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="32"/>
@@ -571,7 +589,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Kosten!$F$3:$F$34</c:f>
+              <c:f>Kosten!$F$4:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -998,7 +1016,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Kosten!$C$3:$C$34</c:f>
+              <c:f>Kosten!$C$4:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1103,7 +1121,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Wärme!$F$3:$F$34</c:f>
+              <c:f>Wärme!$F$4:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1261,7 +1279,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Kosten!$C$3:$C$34</c:f>
+              <c:f>Kosten!$C$4:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1366,7 +1384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Kosten!$F$3:$F$34</c:f>
+              <c:f>Kosten!$F$4:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2858,13 +2876,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2901,13 +2919,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>123826</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>157163</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3201,10 +3219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ABF507-AFCA-496B-A961-3E8F7099BD5D}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F34"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,35 +3250,11 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43565</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D3" s="4">
-        <v>213</v>
-      </c>
-      <c r="E3" s="5">
-        <v>46.600583999999998</v>
-      </c>
-      <c r="F3">
-        <f>ROUND(E3*($M$4/$M$3),3)</f>
-        <v>6.5910000000000002</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="5">
-        <f>MAX(E3:E34)</f>
-        <v>91.914221999999995</v>
-      </c>
-      <c r="N3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -3270,23 +3264,24 @@
         <v>43565</v>
       </c>
       <c r="C4" s="3">
-        <v>0.21875</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D4" s="4">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" s="5">
-        <v>29.940491000000002</v>
+        <v>46.600583999999998</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F34" si="0">ROUND(E4*($M$4/$M$3),3)</f>
-        <v>4.2350000000000003</v>
+        <f>ROUND(E4*($M$5/$M$4),3)</f>
+        <v>6.5910000000000002</v>
       </c>
       <c r="K4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="M4" s="5">
+        <f>MAX(E4:E35)</f>
+        <v>91.914221999999995</v>
       </c>
       <c r="N4" t="s">
         <v>5</v>
@@ -3300,17 +3295,26 @@
         <v>43565</v>
       </c>
       <c r="C5" s="3">
-        <v>0.22916666666666666</v>
+        <v>0.21875</v>
       </c>
       <c r="D5" s="4">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5" s="5">
-        <v>25.775468</v>
+        <v>29.940491000000002</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>3.6459999999999999</v>
+        <f t="shared" ref="F5:F35" si="0">ROUND(E5*($M$5/$M$4),3)</f>
+        <v>4.2350000000000003</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3321,17 +3325,24 @@
         <v>43565</v>
       </c>
       <c r="C6" s="3">
-        <v>0.23958333333333334</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="D6" s="4">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="5">
-        <v>83.095720999999998</v>
+        <v>25.775468</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>11.753</v>
+        <v>3.6459999999999999</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <f>ROUND(AVERAGE(F4:F35),3)</f>
+        <v>6.468</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3342,17 +3353,17 @@
         <v>43565</v>
       </c>
       <c r="C7" s="3">
-        <v>0.25</v>
+        <v>0.23958333333333334</v>
       </c>
       <c r="D7" s="4">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="5">
-        <v>91.914221999999995</v>
+        <v>83.095720999999998</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11.753</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3363,17 +3374,17 @@
         <v>43565</v>
       </c>
       <c r="C8" s="3">
-        <v>0.26041666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="4">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E8" s="5">
-        <v>35.756607000000002</v>
+        <v>91.914221999999995</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>5.0570000000000004</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3384,10 +3395,10 @@
         <v>43565</v>
       </c>
       <c r="C9" s="3">
-        <v>0.27083333333333331</v>
+        <v>0.26041666666666669</v>
       </c>
       <c r="D9" s="4">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9" s="5">
         <v>35.756607000000002</v>
@@ -3405,17 +3416,17 @@
         <v>43565</v>
       </c>
       <c r="C10" s="3">
-        <v>0.28125</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D10" s="4">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" s="5">
-        <v>30.350949</v>
+        <v>35.756607000000002</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>4.2930000000000001</v>
+        <v>5.0570000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3426,17 +3437,17 @@
         <v>43565</v>
       </c>
       <c r="C11" s="3">
-        <v>0.29166666666666669</v>
+        <v>0.28125</v>
       </c>
       <c r="D11" s="4">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="5">
-        <v>33.848125000000003</v>
+        <v>30.350949</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>4.7869999999999999</v>
+        <v>4.2930000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3447,17 +3458,17 @@
         <v>43565</v>
       </c>
       <c r="C12" s="3">
-        <v>0.30208333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D12" s="4">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12" s="5">
-        <v>51.16339</v>
+        <v>33.848125000000003</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>7.2359999999999998</v>
+        <v>4.7869999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3468,17 +3479,17 @@
         <v>43565</v>
       </c>
       <c r="C13" s="3">
-        <v>0.3125</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="D13" s="4">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E13" s="5">
-        <v>50.210855000000002</v>
+        <v>51.16339</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>7.1020000000000003</v>
+        <v>7.2359999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3489,17 +3500,17 @@
         <v>43565</v>
       </c>
       <c r="C14" s="3">
-        <v>0.32291666666666669</v>
+        <v>0.3125</v>
       </c>
       <c r="D14" s="4">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E14" s="5">
-        <v>36.875371999999999</v>
+        <v>50.210855000000002</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>5.2160000000000002</v>
+        <v>7.1020000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -3510,17 +3521,17 @@
         <v>43565</v>
       </c>
       <c r="C15" s="3">
-        <v>0.33333333333333331</v>
+        <v>0.32291666666666669</v>
       </c>
       <c r="D15" s="4">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E15" s="5">
-        <v>41.473275999999998</v>
+        <v>36.875371999999999</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>5.8659999999999997</v>
+        <v>5.2160000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3531,17 +3542,17 @@
         <v>43565</v>
       </c>
       <c r="C16" s="3">
-        <v>0.34375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D16" s="4">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16" s="5">
-        <v>48.370134</v>
+        <v>41.473275999999998</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>6.8410000000000002</v>
+        <v>5.8659999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3552,17 +3563,17 @@
         <v>43565</v>
       </c>
       <c r="C17" s="3">
-        <v>0.35416666666666669</v>
+        <v>0.34375</v>
       </c>
       <c r="D17" s="4">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E17" s="5">
-        <v>47.835856</v>
+        <v>48.370134</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>6.766</v>
+        <v>6.8410000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3573,17 +3584,17 @@
         <v>43565</v>
       </c>
       <c r="C18" s="3">
-        <v>0.36458333333333331</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D18" s="4">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E18" s="5">
-        <v>46.366593999999999</v>
+        <v>47.835856</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>6.5579999999999998</v>
+        <v>6.766</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,17 +3605,17 @@
         <v>43565</v>
       </c>
       <c r="C19" s="3">
-        <v>0.75</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D19" s="4">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="E19" s="5">
-        <v>32.993085999999998</v>
+        <v>46.366593999999999</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>4.6660000000000004</v>
+        <v>6.5579999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3615,17 +3626,17 @@
         <v>43565</v>
       </c>
       <c r="C20" s="3">
-        <v>0.76041666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="D20" s="4">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E20" s="5">
-        <v>28.714967999999999</v>
+        <v>32.993085999999998</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>4.0609999999999999</v>
+        <v>4.6660000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3636,17 +3647,17 @@
         <v>43565</v>
       </c>
       <c r="C21" s="3">
-        <v>0.77083333333333337</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="D21" s="4">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E21" s="5">
-        <v>33.765253999999999</v>
+        <v>28.714967999999999</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>4.7759999999999998</v>
+        <v>4.0609999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,17 +3668,17 @@
         <v>43565</v>
       </c>
       <c r="C22" s="3">
-        <v>0.78125</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="D22" s="4">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E22" s="5">
-        <v>38.184254000000003</v>
+        <v>33.765253999999999</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>5.4009999999999998</v>
+        <v>4.7759999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3678,17 +3689,17 @@
         <v>43565</v>
       </c>
       <c r="C23" s="3">
-        <v>0.79166666666666663</v>
+        <v>0.78125</v>
       </c>
       <c r="D23" s="4">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E23" s="5">
-        <v>30.779443000000001</v>
+        <v>38.184254000000003</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>4.3529999999999998</v>
+        <v>5.4009999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3699,17 +3710,17 @@
         <v>43565</v>
       </c>
       <c r="C24" s="3">
-        <v>0.80208333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D24" s="4">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E24" s="5">
-        <v>27.077038000000002</v>
+        <v>30.779443000000001</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>3.83</v>
+        <v>4.3529999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3720,17 +3731,17 @@
         <v>43565</v>
       </c>
       <c r="C25" s="3">
-        <v>0.8125</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D25" s="4">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E25" s="5">
-        <v>55.068098999999997</v>
+        <v>27.077038000000002</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>7.7889999999999997</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3741,17 +3752,17 @@
         <v>43565</v>
       </c>
       <c r="C26" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.8125</v>
       </c>
       <c r="D26" s="4">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E26" s="5">
-        <v>65.246667000000002</v>
+        <v>55.068098999999997</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>9.2279999999999998</v>
+        <v>7.7889999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3762,17 +3773,17 @@
         <v>43565</v>
       </c>
       <c r="C27" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="D27" s="4">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E27" s="5">
-        <v>40.252628000000001</v>
+        <v>65.246667000000002</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>5.6929999999999996</v>
+        <v>9.2279999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3783,17 +3794,17 @@
         <v>43565</v>
       </c>
       <c r="C28" s="3">
-        <v>0.84375</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D28" s="4">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E28" s="5">
-        <v>36.407392000000002</v>
+        <v>40.252628000000001</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>5.149</v>
+        <v>5.6929999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3804,17 +3815,17 @@
         <v>43565</v>
       </c>
       <c r="C29" s="3">
-        <v>0.85416666666666663</v>
+        <v>0.84375</v>
       </c>
       <c r="D29" s="4">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E29" s="5">
-        <v>61.822611999999999</v>
+        <v>36.407392000000002</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>8.7439999999999998</v>
+        <v>5.149</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3825,17 +3836,17 @@
         <v>43565</v>
       </c>
       <c r="C30" s="3">
-        <v>0.86458333333333337</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="D30" s="4">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E30" s="5">
-        <v>63.637985</v>
+        <v>61.822611999999999</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>9.0009999999999994</v>
+        <v>8.7439999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3846,17 +3857,17 @@
         <v>43565</v>
       </c>
       <c r="C31" s="3">
-        <v>0.875</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="D31" s="4">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E31" s="5">
-        <v>68.855964</v>
+        <v>63.637985</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>9.7390000000000008</v>
+        <v>9.0009999999999994</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3867,17 +3878,17 @@
         <v>43565</v>
       </c>
       <c r="C32" s="3">
-        <v>0.88541666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="D32" s="4">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E32" s="5">
-        <v>70.160458000000006</v>
+        <v>68.855964</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>9.923</v>
+        <v>9.7390000000000008</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3888,17 +3899,17 @@
         <v>43565</v>
       </c>
       <c r="C33" s="3">
-        <v>0.89583333333333337</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="D33" s="4">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E33" s="5">
-        <v>38.705368999999997</v>
+        <v>70.160458000000006</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>5.4740000000000002</v>
+        <v>9.923</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3909,20 +3920,308 @@
         <v>43565</v>
       </c>
       <c r="C34" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D34" s="4">
+        <v>279</v>
+      </c>
+      <c r="E34" s="5">
+        <v>38.705368999999997</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>5.4740000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2">
+        <v>43565</v>
+      </c>
+      <c r="C35" s="3">
         <v>0.90625</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D35" s="4">
         <v>280</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E35" s="5">
         <v>36.458576999999998</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <f t="shared" si="0"/>
         <v>5.157</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6.5910000000000002</v>
+      </c>
+      <c r="B41">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4.2350000000000003</v>
+      </c>
+      <c r="B42">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3.6459999999999999</v>
+      </c>
+      <c r="B43">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>11.753</v>
+      </c>
+      <c r="B44">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>13</v>
+      </c>
+      <c r="B45">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>5.0570000000000004</v>
+      </c>
+      <c r="B46">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>5.0570000000000004</v>
+      </c>
+      <c r="B47">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4.2930000000000001</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4.7869999999999999</v>
+      </c>
+      <c r="B49">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7.2359999999999998</v>
+      </c>
+      <c r="B50">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>7.1020000000000003</v>
+      </c>
+      <c r="B51">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5.2160000000000002</v>
+      </c>
+      <c r="B52">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5.8659999999999997</v>
+      </c>
+      <c r="B53">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>6.8410000000000002</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>6.766</v>
+      </c>
+      <c r="B55">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>6.5579999999999998</v>
+      </c>
+      <c r="B56">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>4.6660000000000004</v>
+      </c>
+      <c r="B57">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>4.0609999999999999</v>
+      </c>
+      <c r="B58">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>4.7759999999999998</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5.4009999999999998</v>
+      </c>
+      <c r="B60">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>4.3529999999999998</v>
+      </c>
+      <c r="B61">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>3.83</v>
+      </c>
+      <c r="B62">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>7.7889999999999997</v>
+      </c>
+      <c r="B63">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9.2279999999999998</v>
+      </c>
+      <c r="B64">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>5.6929999999999996</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>5.149</v>
+      </c>
+      <c r="B66">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>8.7439999999999998</v>
+      </c>
+      <c r="B67">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>9.0009999999999994</v>
+      </c>
+      <c r="B68">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>9.7390000000000008</v>
+      </c>
+      <c r="B69">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>9.923</v>
+      </c>
+      <c r="B70">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5.4740000000000002</v>
+      </c>
+      <c r="B71">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>5.157</v>
+      </c>
+      <c r="B72">
+        <v>5.3</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A36:C36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3930,10 +4229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAF7B51-A847-4EC9-8F79-6CFAC9CF8371}">
-  <dimension ref="A2:N34"/>
+  <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3945,38 +4244,19 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43565</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D3" s="4">
-        <v>213</v>
-      </c>
-      <c r="E3">
-        <f>$N$4*SIN($N$5*D3+$N$6)+$N$3</f>
-        <v>5.3091875161301241</v>
-      </c>
-      <c r="F3">
-        <f>ROUND(E3,1)</f>
-        <v>5.3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3">
-        <v>4.5</v>
-      </c>
+      <c r="A3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -3986,25 +4266,24 @@
         <v>43565</v>
       </c>
       <c r="C4" s="3">
-        <v>0.21875</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D4" s="4">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E34" si="0">$N$4*SIN($N$5*D4+$N$6)+$N$3</f>
-        <v>5.3713282035709717</v>
+        <f>$N$5*SIN($N$6*D4+$N$7)+$N$4</f>
+        <v>5.3091875161301241</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F34" si="1">ROUND(E4,1)</f>
-        <v>5.4</v>
+        <f>ROUND(E4,1)</f>
+        <v>5.3</v>
       </c>
       <c r="L4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N4">
-        <f>0.2*N3</f>
-        <v>0.9</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4015,24 +4294,25 @@
         <v>43565</v>
       </c>
       <c r="C5" s="3">
-        <v>0.22916666666666666</v>
+        <v>0.21875</v>
       </c>
       <c r="D5" s="4">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>5.3987317851705932</v>
+        <f t="shared" ref="E5:E35" si="0">$N$5*SIN($N$6*D5+$N$7)+$N$4</f>
+        <v>5.3713282035709717</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F5:F35" si="1">ROUND(E5,1)</f>
         <v>5.4</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N5">
-        <v>0.2</v>
+        <f>0.2*N4</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4043,24 +4323,24 @@
         <v>43565</v>
       </c>
       <c r="C6" s="3">
-        <v>0.23958333333333334</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="D6" s="4">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>5.3903057666076153</v>
+        <v>5.3987317851705932</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
         <v>5.4</v>
       </c>
       <c r="L6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N6">
-        <v>2.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4071,18 +4351,24 @@
         <v>43565</v>
       </c>
       <c r="C7" s="3">
-        <v>0.25</v>
+        <v>0.23958333333333334</v>
       </c>
       <c r="D7" s="4">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>5.3463860666523031</v>
+        <v>5.3903057666076153</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>5.3</v>
+        <v>5.4</v>
+      </c>
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4093,19 +4379,26 @@
         <v>43565</v>
       </c>
       <c r="C8" s="3">
-        <v>0.26041666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="4">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>5.2687236251452507</v>
+        <v>5.3463860666523031</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
         <v>5.3</v>
       </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <f>ROUND(AVERAGE(F4:F35),1)</f>
+        <v>4.8</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -4115,18 +4408,18 @@
         <v>43565</v>
       </c>
       <c r="C9" s="3">
-        <v>0.27083333333333331</v>
+        <v>0.26041666666666669</v>
       </c>
       <c r="D9" s="4">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>5.1604145985513323</v>
+        <v>5.2687236251452507</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>5.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4137,18 +4430,18 @@
         <v>43565</v>
       </c>
       <c r="C10" s="3">
-        <v>0.28125</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="D10" s="4">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>5.0257769259719574</v>
+        <v>5.1604145985513323</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4159,18 +4452,18 @@
         <v>43565</v>
       </c>
       <c r="C11" s="3">
-        <v>0.29166666666666669</v>
+        <v>0.28125</v>
       </c>
       <c r="D11" s="4">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>4.8701781865391105</v>
+        <v>5.0257769259719574</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>4.9000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4181,18 +4474,18 @@
         <v>43565</v>
       </c>
       <c r="C12" s="3">
-        <v>0.30208333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D12" s="4">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>4.6998216109737676</v>
+        <v>4.8701781865391105</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4203,18 +4496,18 @@
         <v>43565</v>
       </c>
       <c r="C13" s="3">
-        <v>0.3125</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="D13" s="4">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>4.5214987783524654</v>
+        <v>4.6998216109737676</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4225,18 +4518,18 @@
         <v>43565</v>
       </c>
       <c r="C14" s="3">
-        <v>0.32291666666666669</v>
+        <v>0.3125</v>
       </c>
       <c r="D14" s="4">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>4.342318857281561</v>
+        <v>4.5214987783524654</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4247,18 +4540,18 @@
         <v>43565</v>
       </c>
       <c r="C15" s="3">
-        <v>0.33333333333333331</v>
+        <v>0.32291666666666669</v>
       </c>
       <c r="D15" s="4">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>4.1694251857792279</v>
+        <v>4.342318857281561</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -4269,18 +4562,18 @@
         <v>43565</v>
       </c>
       <c r="C16" s="3">
-        <v>0.34375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D16" s="4">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>4.00971048893072</v>
+        <v>4.1694251857792279</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4291,18 +4584,18 @@
         <v>43565</v>
       </c>
       <c r="C17" s="3">
-        <v>0.35416666666666669</v>
+        <v>0.34375</v>
       </c>
       <c r="D17" s="4">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>3.8695420876905233</v>
+        <v>4.00971048893072</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4313,18 +4606,18 @@
         <v>43565</v>
       </c>
       <c r="C18" s="3">
-        <v>0.36458333333333331</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D18" s="4">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>3.7545080538891193</v>
+        <v>3.8695420876905233</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4335,18 +4628,18 @@
         <v>43565</v>
       </c>
       <c r="C19" s="3">
-        <v>0.75</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D19" s="4">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>3.7199163831653168</v>
+        <v>3.7545080538891193</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4357,18 +4650,18 @@
         <v>43565</v>
       </c>
       <c r="C20" s="3">
-        <v>0.76041666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="D20" s="4">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>3.824639562784105</v>
+        <v>3.7199163831653168</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4379,18 +4672,18 @@
         <v>43565</v>
       </c>
       <c r="C21" s="3">
-        <v>0.77083333333333337</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="D21" s="4">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>3.9562872318115909</v>
+        <v>3.824639562784105</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4401,18 +4694,18 @@
         <v>43565</v>
       </c>
       <c r="C22" s="3">
-        <v>0.78125</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="D22" s="4">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>4.1096110131218841</v>
+        <v>3.9562872318115909</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4423,18 +4716,18 @@
         <v>43565</v>
       </c>
       <c r="C23" s="3">
-        <v>0.79166666666666663</v>
+        <v>0.78125</v>
       </c>
       <c r="D23" s="4">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>4.2784983713953268</v>
+        <v>4.1096110131218841</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4445,18 +4738,18 @@
         <v>43565</v>
       </c>
       <c r="C24" s="3">
-        <v>0.80208333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D24" s="4">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>4.4562163006124216</v>
+        <v>4.2784983713953268</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4467,18 +4760,18 @@
         <v>43565</v>
       </c>
       <c r="C25" s="3">
-        <v>0.8125</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D25" s="4">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>4.6356797477566518</v>
+        <v>4.4562163006124216</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4489,18 +4782,18 @@
         <v>43565</v>
       </c>
       <c r="C26" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.8125</v>
       </c>
       <c r="D26" s="4">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>4.8097340715200287</v>
+        <v>4.6356797477566518</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4511,18 +4804,18 @@
         <v>43565</v>
       </c>
       <c r="C27" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="D27" s="4">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>4.9714402752742792</v>
+        <v>4.8097340715200287</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4533,18 +4826,18 @@
         <v>43565</v>
       </c>
       <c r="C28" s="3">
-        <v>0.84375</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D28" s="4">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>5.1143516429691687</v>
+        <v>4.9714402752742792</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>5.0999999999999996</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4555,18 +4848,18 @@
         <v>43565</v>
       </c>
       <c r="C29" s="3">
-        <v>0.85416666666666663</v>
+        <v>0.84375</v>
       </c>
       <c r="D29" s="4">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>5.2327707493575915</v>
+        <v>5.1143516429691687</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4577,18 +4870,18 @@
         <v>43565</v>
       </c>
       <c r="C30" s="3">
-        <v>0.86458333333333337</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="D30" s="4">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>5.3219765983609486</v>
+        <v>5.2327707493575915</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4599,18 +4892,18 @@
         <v>43565</v>
       </c>
       <c r="C31" s="3">
-        <v>0.875</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="D31" s="4">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>5.3784128342848065</v>
+        <v>5.3219765983609486</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>5.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4621,14 +4914,14 @@
         <v>43565</v>
       </c>
       <c r="C32" s="3">
-        <v>0.88541666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="D32" s="4">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>5.3998295224977229</v>
+        <v>5.3784128342848065</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
@@ -4643,14 +4936,14 @@
         <v>43565</v>
       </c>
       <c r="C33" s="3">
-        <v>0.89583333333333337</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="D33" s="4">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>5.3853728472249172</v>
+        <v>5.3998295224977229</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
@@ -4665,23 +4958,55 @@
         <v>43565</v>
       </c>
       <c r="C34" s="3">
-        <v>0.90625</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="D34" s="4">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>5.3356191504888404</v>
+        <v>5.3853728472249172</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2">
+        <v>43565</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.90625</v>
+      </c>
+      <c r="D35" s="4">
+        <v>280</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>5.3356191504888404</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
         <v>5.3</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>